<commit_message>
Fix duplicate player names by normalizing diacritics (Jokić→Jokic, Dončić→Doncic)
</commit_message>
<xml_diff>
--- a/Most_Recent_Games_Master.xlsx
+++ b/Most_Recent_Games_Master.xlsx
@@ -698,7 +698,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jay Huff</t>
+          <t>Myron Gardner</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -708,12 +708,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -723,12 +723,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>15/7/2/2/2</t>
+          <t>10/7/6/2/0</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>PTS 11-15 | REB 6-10 | AST 0-2 | STL 2-3 | BLK 2-3</t>
+          <t>PTS 6-10 | REB 6-10 | AST 6-8 | STL 2-3 | BLK 0-1</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -741,7 +741,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Myron Gardner</t>
+          <t>Jay Huff</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -751,12 +751,12 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -766,25 +766,25 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>10/7/6/2/0</t>
+          <t>15/7/2/2/2</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>PTS 6-10 | REB 6-10 | AST 6-8 | STL 2-3 | BLK 0-1</t>
+          <t>PTS 11-15 | REB 6-10 | AST 0-2 | STL 2-3 | BLK 2-3</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2231</v>
+        <v>0.2466</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kasparas Jakučionis</t>
+          <t>Kasparas Jakucionis</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -818,10 +818,10 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1003</v>
+        <v>0.1108</v>
       </c>
     </row>
     <row r="10">
@@ -861,10 +861,10 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I10" t="n">
-        <v>0.08210000000000001</v>
+        <v>0.1108</v>
       </c>
     </row>
     <row r="11">
@@ -947,16 +947,16 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0273</v>
+        <v>0.0302</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Jalen Brunson</t>
+          <t>Alex Sarr</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -966,12 +966,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -981,25 +981,25 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>31/3/8/0/0</t>
+          <t>12/12/5/1/0</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>PTS 31-40 | REB 3-5 | AST 6-8 | STL 0-1 | BLK 0-1</t>
+          <t>PTS 11-15 | REB 11-15 | AST 3-5 | STL 0-1 | BLK 0-1</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" t="n">
-        <v>0.0247</v>
+        <v>0.0273</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Kel'el Ware</t>
+          <t>Jalen Brunson</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1009,12 +1009,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1024,25 +1024,25 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>19/14/1/0/1</t>
+          <t>31/3/8/0/0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>PTS 16-20 | REB 11-15 | AST 0-2 | STL 0-1 | BLK 0-1</t>
+          <t>PTS 31-40 | REB 3-5 | AST 6-8 | STL 0-1 | BLK 0-1</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0224</v>
+        <v>0.0273</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Alex Sarr</t>
+          <t>Kel'el Ware</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1052,14 +1052,14 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>WAS</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>MIA</t>
-        </is>
-      </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>2025-26</t>
@@ -1067,19 +1067,19 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>12/12/5/1/0</t>
+          <t>19/14/1/0/1</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>PTS 11-15 | REB 11-15 | AST 3-5 | STL 0-1 | BLK 0-1</t>
+          <t>PTS 16-20 | REB 11-15 | AST 0-2 | STL 0-1 | BLK 0-1</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="I15" t="n">
-        <v>0.0166</v>
+        <v>0.0247</v>
       </c>
     </row>
     <row r="16">
@@ -1162,10 +1162,10 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0045</v>
+        <v>0.0055</v>
       </c>
     </row>
     <row r="18">
@@ -1205,10 +1205,10 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0033</v>
+        <v>0.0041</v>
       </c>
     </row>
     <row r="19">
@@ -1248,10 +1248,10 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0033</v>
+        <v>0.0041</v>
       </c>
     </row>
     <row r="20">
@@ -1291,16 +1291,16 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I20" t="n">
-        <v>0.0018</v>
+        <v>0.0022</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Immanuel Quickley</t>
+          <t>Norman Powell</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1310,12 +1310,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1325,25 +1325,25 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>13/4/6/1/0</t>
+          <t>21/4/0/1/0</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>PTS 11-15 | REB 3-5 | AST 6-8 | STL 0-1 | BLK 0-1</t>
+          <t>PTS 21-25 | REB 3-5 | AST 0-2 | STL 0-1 | BLK 0-1</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0005</v>
+        <v>0.0005999999999999999</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Norman Powell</t>
+          <t>Immanuel Quickley</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1353,12 +1353,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1368,19 +1368,19 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>21/4/0/1/0</t>
+          <t>13/4/6/1/0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>PTS 21-25 | REB 3-5 | AST 0-2 | STL 0-1 | BLK 0-1</t>
+          <t>PTS 11-15 | REB 3-5 | AST 6-8 | STL 0-1 | BLK 0-1</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I22" t="n">
-        <v>0.0004</v>
+        <v>0.0005</v>
       </c>
     </row>
     <row r="23">
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I23" t="n">
         <v>0.0003</v>
@@ -1429,7 +1429,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Simone Fontecchio</t>
+          <t>Jose Alvarado</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1439,12 +1439,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1454,19 +1454,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>12/5/3/3/0</t>
+          <t>12/2/2/2/1</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>PTS 11-15 | REB 3-5 | AST 3-5 | STL 2-3 | BLK 0-1</t>
+          <t>PTS 11-15 | REB 0-2 | AST 0-2 | STL 2-3 | BLK 0-1</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0002</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="25">
@@ -1506,16 +1506,16 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I25" t="n">
-        <v>0.0002</v>
+        <v>0.0003</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Jose Alvarado</t>
+          <t>Simone Fontecchio</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1525,12 +1525,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1540,16 +1540,16 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>12/2/2/2/1</t>
+          <t>12/5/3/3/0</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>PTS 11-15 | REB 0-2 | AST 0-2 | STL 2-3 | BLK 0-1</t>
+          <t>PTS 11-15 | REB 3-5 | AST 3-5 | STL 2-3 | BLK 0-1</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I26" t="n">
         <v>0.0002</v>
@@ -1592,16 +1592,16 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0001</v>
+        <v>0.0002</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Jonathan Mogbo</t>
+          <t>Jahmir Young</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1611,12 +1611,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>0/0/0/0/0</t>
+          <t>2/1/0/0/0</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1635,7 +1635,7 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -1644,7 +1644,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Enrique Freeman</t>
+          <t>Keshon Gilbert</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1654,12 +1654,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1669,7 +1669,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>0/2/0/0/0</t>
+          <t>0/1/1/0/1</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1678,7 +1678,7 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I29" t="n">
         <v>0</v>
@@ -1687,7 +1687,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Joan Beringer</t>
+          <t>Dru Smith</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1697,12 +1697,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>4/1/1/0/1</t>
+          <t>0/1/2/1/0</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1721,7 +1721,7 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I30" t="n">
         <v>0</v>
@@ -1730,7 +1730,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Jamison Battle</t>
+          <t>Nikola Jovic</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1740,12 +1740,12 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>0/2/0/0/0</t>
+          <t>4/1/2/1/0</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I31" t="n">
         <v>0</v>
@@ -1773,7 +1773,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Collin Murray-Boyles</t>
+          <t>Trey Jemison III</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1783,12 +1783,12 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2/0/0/0/1</t>
+          <t>0/1/0/0/0</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I32" t="n">
         <v>0</v>
@@ -1816,7 +1816,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Joe Ingles</t>
+          <t>Pacome Dadiet</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1826,12 +1826,12 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>0/1/2/0/0</t>
+          <t>0/2/1/0/0</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1850,7 +1850,7 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I33" t="n">
         <v>0</v>
@@ -1859,7 +1859,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Julian Phillips</t>
+          <t>Jordan Clarkson</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1869,12 +1869,12 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1884,7 +1884,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2/0/0/0/0</t>
+          <t>0/2/1/0/1</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1893,7 +1893,7 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I34" t="n">
         <v>0</v>
@@ -1902,7 +1902,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Cam Christie</t>
+          <t>Kevin McCullar Jr.</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1912,12 +1912,12 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2/0/1/0/0</t>
+          <t>0/0/0/0/0</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1936,7 +1936,7 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I35" t="n">
         <v>0</v>
@@ -1945,7 +1945,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Jaden McDaniels</t>
+          <t>Hugo Gonzalez</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1955,12 +1955,12 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1970,7 +1970,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2/2/0/1/0</t>
+          <t>2/1/0/0/0</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1979,7 +1979,7 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I36" t="n">
         <v>0</v>
@@ -1988,7 +1988,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Dalano Banton</t>
+          <t>Amari Williams</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1998,12 +1998,12 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2/0/0/0/0</t>
+          <t>0/2/0/0/0</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="H37" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I37" t="n">
         <v>0</v>
@@ -2031,7 +2031,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>A.J. Lawson</t>
+          <t>Ariel Hukporti</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2041,12 +2041,12 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -2056,7 +2056,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>0/1/0/0/0</t>
+          <t>0/0/0/0/0</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="H38" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I38" t="n">
         <v>0</v>
@@ -2074,7 +2074,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Alijah Martin</t>
+          <t>Jonathan Mogbo</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2099,7 +2099,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2/1/0/1/0</t>
+          <t>0/0/0/0/0</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -2108,7 +2108,7 @@
         </is>
       </c>
       <c r="H39" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
@@ -2117,7 +2117,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Jahmir Young</t>
+          <t>Enrique Freeman</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2127,12 +2127,12 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -2142,7 +2142,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2/1/0/0/0</t>
+          <t>0/2/0/0/0</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -2151,7 +2151,7 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I40" t="n">
         <v>0</v>
@@ -2160,7 +2160,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Keshon Gilbert</t>
+          <t>Joan Beringer</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2170,12 +2170,12 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -2185,7 +2185,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>0/1/1/0/1</t>
+          <t>4/1/1/0/1</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2194,7 +2194,7 @@
         </is>
       </c>
       <c r="H41" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I41" t="n">
         <v>0</v>
@@ -2203,7 +2203,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Dru Smith</t>
+          <t>Jamison Battle</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2213,12 +2213,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -2228,7 +2228,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>0/1/2/1/0</t>
+          <t>0/2/0/0/0</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2237,7 +2237,7 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I42" t="n">
         <v>0</v>
@@ -2246,7 +2246,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Nikola Jović</t>
+          <t>Collin Murray-Boyles</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2256,12 +2256,12 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>4/1/2/1/0</t>
+          <t>2/0/0/0/1</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
@@ -2280,7 +2280,7 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I43" t="n">
         <v>0</v>
@@ -2289,7 +2289,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Trey Jemison III</t>
+          <t>Joe Ingles</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2299,12 +2299,12 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0/1/0/0/0</t>
+          <t>0/1/2/0/0</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2323,7 +2323,7 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I44" t="n">
         <v>0</v>
@@ -2332,7 +2332,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Pacôme Dadiet</t>
+          <t>Julian Phillips</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2342,12 +2342,12 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0/2/1/0/0</t>
+          <t>2/0/0/0/0</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2366,7 +2366,7 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I45" t="n">
         <v>0</v>
@@ -2375,7 +2375,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Jordan Clarkson</t>
+          <t>Cam Christie</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2385,12 +2385,12 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2400,7 +2400,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>0/2/1/0/1</t>
+          <t>2/0/1/0/0</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2409,7 +2409,7 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I46" t="n">
         <v>0</v>
@@ -2418,7 +2418,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Kevin McCullar Jr.</t>
+          <t>Jaden McDaniels</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2428,12 +2428,12 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2443,7 +2443,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>0/0/0/0/0</t>
+          <t>2/2/0/1/0</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I47" t="n">
         <v>0</v>
@@ -2461,7 +2461,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Hugo González</t>
+          <t>Dalano Banton</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2471,12 +2471,12 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2/1/0/0/0</t>
+          <t>2/0/0/0/0</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2495,7 +2495,7 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I48" t="n">
         <v>0</v>
@@ -2504,7 +2504,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Amari Williams</t>
+          <t>A.J. Lawson</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2514,12 +2514,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -2529,7 +2529,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>0/2/0/0/0</t>
+          <t>0/1/0/0/0</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2538,7 +2538,7 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I49" t="n">
         <v>0</v>
@@ -2547,7 +2547,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Ariel Hukporti</t>
+          <t>Alijah Martin</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2557,12 +2557,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>0/0/0/0/0</t>
+          <t>2/1/0/1/0</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2581,7 +2581,7 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>6816</v>
+        <v>6697</v>
       </c>
       <c r="I50" t="n">
         <v>0</v>
@@ -2590,7 +2590,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Kam Jones</t>
+          <t>Will Riley</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2600,12 +2600,12 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -2615,7 +2615,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>7/1/1/0/0</t>
+          <t>9/1/0/1/1</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2624,7 +2624,7 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>794</v>
+        <v>772</v>
       </c>
       <c r="I51" t="n">
         <v>0</v>
@@ -2633,7 +2633,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Jaylen Clark</t>
+          <t>Tyler Kolek</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2643,12 +2643,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>8/1/0/1/0</t>
+          <t>6/0/0/0/0</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2667,7 +2667,7 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>794</v>
+        <v>772</v>
       </c>
       <c r="I52" t="n">
         <v>0</v>
@@ -2676,7 +2676,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Bones Hyland</t>
+          <t>Kam Jones</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2686,12 +2686,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>10/1/2/0/0</t>
+          <t>7/1/1/0/0</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
@@ -2710,7 +2710,7 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>794</v>
+        <v>772</v>
       </c>
       <c r="I53" t="n">
         <v>0</v>
@@ -2719,7 +2719,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Aaron Nesmith</t>
+          <t>Jaylen Clark</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2729,12 +2729,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -2744,7 +2744,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>7/1/1/1/0</t>
+          <t>8/1/0/1/0</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2753,7 +2753,7 @@
         </is>
       </c>
       <c r="H54" t="n">
-        <v>794</v>
+        <v>772</v>
       </c>
       <c r="I54" t="n">
         <v>0</v>
@@ -2762,7 +2762,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Will Riley</t>
+          <t>Bones Hyland</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2772,12 +2772,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>9/1/0/1/1</t>
+          <t>10/1/2/0/0</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2796,7 +2796,7 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>794</v>
+        <v>772</v>
       </c>
       <c r="I55" t="n">
         <v>0</v>
@@ -2805,7 +2805,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Tyler Kolek</t>
+          <t>Aaron Nesmith</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2815,12 +2815,12 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -2830,7 +2830,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>6/0/0/0/0</t>
+          <t>7/1/1/1/0</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2839,7 +2839,7 @@
         </is>
       </c>
       <c r="H56" t="n">
-        <v>794</v>
+        <v>772</v>
       </c>
       <c r="I56" t="n">
         <v>0</v>
@@ -2848,7 +2848,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Jamal Shead</t>
+          <t>Sharife Cooper</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2858,12 +2858,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>6/0/4/0/0</t>
+          <t>8/1/3/1/0</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="I57" t="n">
         <v>0</v>
@@ -2891,7 +2891,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Jordan Miller</t>
+          <t>Jamal Shead</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2901,12 +2901,12 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2916,7 +2916,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>8/1/4/0/0</t>
+          <t>6/0/4/0/0</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
@@ -2925,7 +2925,7 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="I58" t="n">
         <v>0</v>
@@ -2934,7 +2934,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Sharife Cooper</t>
+          <t>Jordan Miller</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2944,12 +2944,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2959,7 +2959,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>8/1/3/1/0</t>
+          <t>8/1/4/0/0</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2968,7 +2968,7 @@
         </is>
       </c>
       <c r="H59" t="n">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="I59" t="n">
         <v>0</v>
@@ -2977,7 +2977,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>John Collins</t>
+          <t>Tristan Vukcevic</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2987,12 +2987,12 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>15/4/0/1/1</t>
+          <t>14/5/2/0/0</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
@@ -3011,7 +3011,7 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I60" t="n">
         <v>0</v>
@@ -3020,7 +3020,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Tristan Vukcevic</t>
+          <t>Mikal Bridges</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3030,12 +3030,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>14/5/2/0/0</t>
+          <t>14/4/1/0/1</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
@@ -3054,7 +3054,7 @@
         </is>
       </c>
       <c r="H61" t="n">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I61" t="n">
         <v>0</v>
@@ -3063,7 +3063,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Mikal Bridges</t>
+          <t>John Collins</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -3073,12 +3073,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -3088,7 +3088,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>14/4/1/0/1</t>
+          <t>15/4/0/1/1</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
@@ -3097,7 +3097,7 @@
         </is>
       </c>
       <c r="H62" t="n">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="I62" t="n">
         <v>0</v>
@@ -3140,7 +3140,7 @@
         </is>
       </c>
       <c r="H63" t="n">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="I63" t="n">
         <v>0</v>
@@ -3183,7 +3183,7 @@
         </is>
       </c>
       <c r="H64" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="I64" t="n">
         <v>0</v>
@@ -3192,7 +3192,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Jarace Walker</t>
+          <t>Justin Champagnie</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -3202,12 +3202,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -3217,7 +3217,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>13/6/2/1/0</t>
+          <t>13/7/1/1/0</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
@@ -3226,7 +3226,7 @@
         </is>
       </c>
       <c r="H65" t="n">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="I65" t="n">
         <v>0</v>
@@ -3235,7 +3235,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Yanic Konan Niederhäuser</t>
+          <t>Nikola Vucevic</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -3245,12 +3245,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>15/6/2/0/1</t>
+          <t>11/6/0/0/1</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -3269,7 +3269,7 @@
         </is>
       </c>
       <c r="H66" t="n">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="I66" t="n">
         <v>0</v>
@@ -3278,7 +3278,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Justin Champagnie</t>
+          <t>Karl-Anthony Towns</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -3288,12 +3288,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -3303,7 +3303,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>13/7/1/1/0</t>
+          <t>11/10/1/1/0</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="H67" t="n">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="I67" t="n">
         <v>0</v>
@@ -3321,7 +3321,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Nikola Vučević</t>
+          <t>Jarace Walker</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -3331,12 +3331,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -3346,7 +3346,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>11/6/0/0/1</t>
+          <t>13/6/2/1/0</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -3355,7 +3355,7 @@
         </is>
       </c>
       <c r="H68" t="n">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="I68" t="n">
         <v>0</v>
@@ -3364,7 +3364,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Karl-Anthony Towns</t>
+          <t>Yanic Konan Niederhauser</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -3374,12 +3374,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -3389,7 +3389,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>11/10/1/1/0</t>
+          <t>15/6/2/0/1</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
@@ -3398,7 +3398,7 @@
         </is>
       </c>
       <c r="H69" t="n">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="I69" t="n">
         <v>0</v>
@@ -3441,7 +3441,7 @@
         </is>
       </c>
       <c r="H70" t="n">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="I70" t="n">
         <v>0</v>
@@ -3484,7 +3484,7 @@
         </is>
       </c>
       <c r="H71" t="n">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="I71" t="n">
         <v>0</v>
@@ -3527,7 +3527,7 @@
         </is>
       </c>
       <c r="H72" t="n">
-        <v>379</v>
+        <v>359</v>
       </c>
       <c r="I72" t="n">
         <v>0</v>
@@ -3570,7 +3570,7 @@
         </is>
       </c>
       <c r="H73" t="n">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="I73" t="n">
         <v>0</v>
@@ -3613,7 +3613,7 @@
         </is>
       </c>
       <c r="H74" t="n">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="I74" t="n">
         <v>0</v>
@@ -3622,7 +3622,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Kobe Sanders</t>
+          <t>Bilal Coulibaly</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3632,12 +3632,12 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -3647,7 +3647,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>10/4/2/0/0</t>
+          <t>7/4/1/1/1</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -3656,7 +3656,7 @@
         </is>
       </c>
       <c r="H75" t="n">
-        <v>739</v>
+        <v>713</v>
       </c>
       <c r="I75" t="n">
         <v>0</v>
@@ -3665,7 +3665,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Bilal Coulibaly</t>
+          <t>Mohamed Diawara</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3675,12 +3675,12 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>7/4/1/1/1</t>
+          <t>10/3/1/1/0</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
@@ -3699,7 +3699,7 @@
         </is>
       </c>
       <c r="H76" t="n">
-        <v>739</v>
+        <v>713</v>
       </c>
       <c r="I76" t="n">
         <v>0</v>
@@ -3708,7 +3708,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Mohamed Diawara</t>
+          <t>Luka Garza</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3718,14 +3718,14 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
+          <t>BOS</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
           <t>NYK</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>BOS</t>
-        </is>
-      </c>
       <c r="E77" t="inlineStr">
         <is>
           <t>2025-26</t>
@@ -3733,7 +3733,7 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>10/3/1/1/0</t>
+          <t>6/3/0/0/0</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
@@ -3742,7 +3742,7 @@
         </is>
       </c>
       <c r="H77" t="n">
-        <v>739</v>
+        <v>713</v>
       </c>
       <c r="I77" t="n">
         <v>0</v>
@@ -3751,7 +3751,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Luka Garza</t>
+          <t>Kobe Sanders</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3761,12 +3761,12 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>6/3/0/0/0</t>
+          <t>10/4/2/0/0</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3785,7 +3785,7 @@
         </is>
       </c>
       <c r="H78" t="n">
-        <v>739</v>
+        <v>713</v>
       </c>
       <c r="I78" t="n">
         <v>0</v>
@@ -3828,7 +3828,7 @@
         </is>
       </c>
       <c r="H79" t="n">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="I79" t="n">
         <v>0</v>
@@ -3871,7 +3871,7 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="I80" t="n">
         <v>0</v>
@@ -3914,7 +3914,7 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="I81" t="n">
         <v>0</v>
@@ -3923,7 +3923,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Nicolas Batum</t>
+          <t>Neemias Queta</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3933,12 +3933,12 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -3948,7 +3948,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>3/3/0/0/0</t>
+          <t>4/5/1/0/0</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3957,7 +3957,7 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>1020</v>
+        <v>977</v>
       </c>
       <c r="I82" t="n">
         <v>0</v>
@@ -3966,7 +3966,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Donte DiVincenzo</t>
+          <t>Ron Harper Jr.</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3976,12 +3976,12 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>1/4/2/1/0</t>
+          <t>3/3/0/0/1</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -4000,7 +4000,7 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>1020</v>
+        <v>977</v>
       </c>
       <c r="I83" t="n">
         <v>0</v>
@@ -4009,7 +4009,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Neemias Queta</t>
+          <t>Nicolas Batum</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -4019,12 +4019,12 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -4034,7 +4034,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>4/5/1/0/0</t>
+          <t>3/3/0/0/0</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -4043,7 +4043,7 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>1020</v>
+        <v>977</v>
       </c>
       <c r="I84" t="n">
         <v>0</v>
@@ -4052,7 +4052,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Ron Harper Jr.</t>
+          <t>Donte DiVincenzo</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -4062,12 +4062,12 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -4077,7 +4077,7 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>3/3/0/0/1</t>
+          <t>1/4/2/1/0</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
@@ -4086,7 +4086,7 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>1020</v>
+        <v>977</v>
       </c>
       <c r="I85" t="n">
         <v>0</v>
@@ -4095,7 +4095,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Johnny Furphy</t>
+          <t>Davion Mitchell</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -4105,12 +4105,12 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -4120,7 +4120,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>4/2/3/0/0</t>
+          <t>5/2/3/1/0</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -4129,7 +4129,7 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="I86" t="n">
         <v>0</v>
@@ -4138,7 +4138,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Davion Mitchell</t>
+          <t>Johnny Furphy</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -4148,12 +4148,12 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>5/2/3/1/0</t>
+          <t>4/2/3/0/0</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -4172,7 +4172,7 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="I87" t="n">
         <v>0</v>
@@ -4215,7 +4215,7 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I88" t="n">
         <v>0</v>
@@ -4258,7 +4258,7 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I89" t="n">
         <v>0</v>
@@ -4301,7 +4301,7 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="I90" t="n">
         <v>0</v>
@@ -4344,7 +4344,7 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I91" t="n">
         <v>0</v>
@@ -4387,7 +4387,7 @@
         </is>
       </c>
       <c r="H92" t="n">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I92" t="n">
         <v>0</v>
@@ -4430,7 +4430,7 @@
         </is>
       </c>
       <c r="H93" t="n">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I93" t="n">
         <v>0</v>
@@ -4439,7 +4439,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>RJ Barrett</t>
+          <t>Josh Hart</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -4449,12 +4449,12 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -4464,7 +4464,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>20/8/5/1/0</t>
+          <t>19/6/3/0/0</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -4473,7 +4473,7 @@
         </is>
       </c>
       <c r="H94" t="n">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I94" t="n">
         <v>0</v>
@@ -4482,7 +4482,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Josh Hart</t>
+          <t>RJ Barrett</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -4492,12 +4492,12 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -4507,7 +4507,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>19/6/3/0/0</t>
+          <t>20/8/5/1/0</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -4516,7 +4516,7 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I95" t="n">
         <v>0</v>
@@ -4559,7 +4559,7 @@
         </is>
       </c>
       <c r="H96" t="n">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I96" t="n">
         <v>0</v>
@@ -4602,7 +4602,7 @@
         </is>
       </c>
       <c r="H97" t="n">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I97" t="n">
         <v>0</v>

</xml_diff>